<commit_message>
created barchart in budget page
</commit_message>
<xml_diff>
--- a/src/main/resources/userfiles/test/test_bankstatement.xlsx
+++ b/src/main/resources/userfiles/test/test_bankstatement.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="17">
   <si>
     <t>Category</t>
   </si>
@@ -29,19 +29,40 @@
     <t>Account</t>
   </si>
   <si>
-    <t>Transportation</t>
+    <t>Food</t>
+  </si>
+  <si>
+    <t>asdwa</t>
+  </si>
+  <si>
+    <t>2023-03-20</t>
+  </si>
+  <si>
+    <t>432.0</t>
+  </si>
+  <si>
+    <t>Savings</t>
+  </si>
+  <si>
+    <t>sdaw</t>
+  </si>
+  <si>
+    <t>2023-03-23</t>
+  </si>
+  <si>
+    <t>dwads</t>
+  </si>
+  <si>
+    <t>2023-03-01</t>
+  </si>
+  <si>
+    <t>43.0</t>
   </si>
   <si>
     <t>dwas</t>
   </si>
   <si>
-    <t>2023-03-22</t>
-  </si>
-  <si>
-    <t>123.0</t>
-  </si>
-  <si>
-    <t>Checkings</t>
+    <t>2023-03-02</t>
   </si>
 </sst>
 </file>
@@ -86,7 +107,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -126,6 +147,57 @@
         <v>9</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>